<commit_message>
add more feature and todo (proxy tabs)
</commit_message>
<xml_diff>
--- a/db/information.xlsx
+++ b/db/information.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -413,60 +413,63 @@
         <v>os</v>
       </c>
       <c r="D1" t="str">
+        <v>userAgent</v>
+      </c>
+      <c r="E1" t="str">
+        <v>screen</v>
+      </c>
+      <c r="F1" t="str">
+        <v>cpu</v>
+      </c>
+      <c r="G1" t="str">
+        <v>languages</v>
+      </c>
+      <c r="H1" t="str">
+        <v>startURL</v>
+      </c>
+      <c r="I1" t="str">
+        <v>delayOpenSeconds</v>
+      </c>
+      <c r="J1" t="str">
+        <v>webRTC</v>
+      </c>
+      <c r="K1" t="str">
+        <v>getlocation</v>
+      </c>
+      <c r="L1" t="str">
+        <v>timeZone</v>
+      </c>
+      <c r="M1" t="str">
+        <v>clientRects</v>
+      </c>
+      <c r="N1" t="str">
+        <v>audioContext</v>
+      </c>
+      <c r="O1" t="str">
+        <v>fonts</v>
+      </c>
+      <c r="P1" t="str">
+        <v>isRunning</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>created</v>
+      </c>
+      <c r="R1" t="str">
+        <v>id</v>
+      </c>
+      <c r="S1" t="str">
         <v>version</v>
       </c>
-      <c r="E1" t="str">
-        <v>userAgent</v>
-      </c>
-      <c r="F1" t="str">
-        <v>screen</v>
-      </c>
-      <c r="G1" t="str">
-        <v>cpu</v>
-      </c>
-      <c r="H1" t="str">
-        <v>languages</v>
-      </c>
-      <c r="I1" t="str">
-        <v>startURL</v>
-      </c>
-      <c r="J1" t="str">
-        <v>delayOpenSeconds</v>
-      </c>
-      <c r="K1" t="str">
-        <v>webRTC</v>
-      </c>
-      <c r="L1" t="str">
-        <v>getlocation</v>
-      </c>
-      <c r="M1" t="str">
-        <v>timeZone</v>
-      </c>
-      <c r="N1" t="str">
-        <v>clientRects</v>
-      </c>
-      <c r="O1" t="str">
-        <v>audioContext</v>
-      </c>
-      <c r="P1" t="str">
-        <v>fonts</v>
-      </c>
-      <c r="Q1" t="str">
-        <v>isRunning</v>
-      </c>
-      <c r="R1" t="str">
-        <v>created</v>
-      </c>
-      <c r="S1" t="str">
+      <c r="T1" t="str">
         <v>pathSave</v>
       </c>
-      <c r="T1" t="str">
+      <c r="U1" t="str">
         <v>proxy</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Cuong mm</v>
+        <v>Cuong KK9</v>
       </c>
       <c r="B2" t="str">
         <v>chrome</v>
@@ -474,35 +477,35 @@
       <c r="C2" t="str">
         <v/>
       </c>
-      <c r="D2">
-        <v>130</v>
+      <c r="D2" t="str">
+        <v>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/132.0.0.0 Safari/537.36</v>
       </c>
       <c r="E2" t="str">
-        <v>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/132.0.0.0 Safari/537.36</v>
-      </c>
-      <c r="F2" t="str">
         <v>1920x1080</v>
       </c>
-      <c r="G2">
+      <c r="F2">
         <v>4</v>
       </c>
+      <c r="G2" t="str">
+        <v>vn</v>
+      </c>
       <c r="H2" t="str">
-        <v>vn</v>
-      </c>
-      <c r="I2" t="str">
         <v/>
       </c>
-      <c r="J2">
+      <c r="I2">
         <v>0</v>
       </c>
+      <c r="J2" t="str">
+        <v>real</v>
+      </c>
       <c r="K2" t="str">
-        <v>real</v>
+        <v>prompt</v>
       </c>
       <c r="L2" t="str">
-        <v>prompt</v>
+        <v/>
       </c>
       <c r="M2" t="str">
-        <v/>
+        <v>off</v>
       </c>
       <c r="N2" t="str">
         <v>off</v>
@@ -510,22 +513,25 @@
       <c r="O2" t="str">
         <v>off</v>
       </c>
-      <c r="P2" t="str">
-        <v>off</v>
-      </c>
-      <c r="Q2" t="b">
+      <c r="P2" t="b">
         <v>0</v>
       </c>
+      <c r="Q2" t="str">
+        <v>15:10 7/2/25</v>
+      </c>
       <c r="R2" t="str">
-        <v>09:47 6/2/25</v>
-      </c>
-      <c r="S2" t="str">
-        <v>E:\cuong-mmo\chromeProfile\Cuong mm</v>
+        <v>e5640726-544d-4243-9c2e-f51bf95df8a8</v>
+      </c>
+      <c r="S2">
+        <v>130</v>
+      </c>
+      <c r="T2" t="str">
+        <v>E:\cuong-mmo\chromeProfile\Cuong KK9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Cuong mm 1</v>
+        <v>PHY 99</v>
       </c>
       <c r="B3" t="str">
         <v>chrome</v>
@@ -533,35 +539,35 @@
       <c r="C3" t="str">
         <v/>
       </c>
-      <c r="D3">
-        <v>130</v>
+      <c r="D3" t="str">
+        <v>Mozilla/5.0 (Windows NT 6.1; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/107.0.5304.107 Safari/537.36</v>
       </c>
       <c r="E3" t="str">
-        <v>Mozilla/5.0 (Windows NT 6.1; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/102.0.5005.115 Safari/537.36</v>
-      </c>
-      <c r="F3" t="str">
         <v>1920x1080</v>
       </c>
-      <c r="G3">
+      <c r="F3">
         <v>4</v>
       </c>
+      <c r="G3" t="str">
+        <v>vn</v>
+      </c>
       <c r="H3" t="str">
-        <v>vn</v>
-      </c>
-      <c r="I3" t="str">
+        <v>http://zingnews.vn</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="str">
+        <v>real</v>
+      </c>
+      <c r="K3" t="str">
+        <v>prompt</v>
+      </c>
+      <c r="L3" t="str">
         <v/>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3" t="str">
-        <v>real</v>
-      </c>
-      <c r="L3" t="str">
-        <v>prompt</v>
-      </c>
       <c r="M3" t="str">
-        <v/>
+        <v>off</v>
       </c>
       <c r="N3" t="str">
         <v>off</v>
@@ -569,22 +575,25 @@
       <c r="O3" t="str">
         <v>off</v>
       </c>
-      <c r="P3" t="str">
-        <v>off</v>
-      </c>
-      <c r="Q3" t="b">
+      <c r="P3" t="b">
         <v>0</v>
       </c>
+      <c r="Q3" t="str">
+        <v>15:10 7/2/25</v>
+      </c>
       <c r="R3" t="str">
-        <v>09:47 6/2/25</v>
-      </c>
-      <c r="S3" t="str">
-        <v>E:\cuong-mmo\chromeProfile\Cuong mm 1</v>
+        <v>dc0cdacb-e42b-4a60-8cfd-1d40dd65048a</v>
+      </c>
+      <c r="S3">
+        <v>130</v>
+      </c>
+      <c r="T3" t="str">
+        <v>E:\cuong-mmo\chromeProfile\PHY 99</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:T3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:U3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>